<commit_message>
New code with pre-build google sheet
</commit_message>
<xml_diff>
--- a/TesteReal1.xlsx
+++ b/TesteReal1.xlsx
@@ -1,90 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rico/Documents/Kali_and_cmds/Python/Whats automacao/WhatsAppBot/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13107EA-2E50-E343-B3D5-528897E4D8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-34720" yWindow="-1300" windowWidth="28040" windowHeight="16540" xr2:uid="{096B859E-EAF3-544D-B856-ADC316462FA5}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="16540" windowWidth="28040" xWindow="-34720" yWindow="-1300"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Nome</t>
-  </si>
-  <si>
-    <t>Numero</t>
-  </si>
-  <si>
-    <t>Marca</t>
-  </si>
-  <si>
-    <t>Modelo</t>
-  </si>
-  <si>
-    <t>que é bom nada ne</t>
-  </si>
-  <si>
-    <t>nao sei</t>
-  </si>
-  <si>
-    <t>Mensagem</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <sz val="8"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -100,16 +52,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -123,21 +75,81 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook r:id="rId1">
     <sheetNames>
       <sheetName val="Servico Dados"/>
       <sheetName val="Fernanda"/>
@@ -480,97 +492,116 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9D96EAC-1AD8-2E4C-BB21-38933F905487}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="12.5" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" customWidth="1"/>
-    <col min="4" max="4" width="16.5" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" width="12.5"/>
+    <col customWidth="1" max="2" min="2" width="11.6640625"/>
+    <col customWidth="1" max="3" min="3" width="17.83203125"/>
+    <col customWidth="1" max="4" min="4" width="16.5"/>
+    <col customWidth="1" max="5" min="5" width="13.6640625"/>
+    <col customWidth="1" max="6" min="6" width="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Data</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Numero</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Marca</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Modelo</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Mensagem</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" s="1">
         <f>[1]Fernanda!X2</f>
-        <v>44440</v>
-      </c>
-      <c r="B2" t="str">
+        <v/>
+      </c>
+      <c r="B2">
         <f>[1]Fernanda!Z2</f>
-        <v>LUIZ</v>
-      </c>
-      <c r="C2" s="3">
+        <v/>
+      </c>
+      <c r="C2" s="3" t="n">
         <v>5544988045037</v>
       </c>
-      <c r="D2" t="str">
+      <c r="D2">
         <f>[1]Fernanda!AB2</f>
-        <v>HONDA</v>
-      </c>
-      <c r="E2" s="2" t="str">
+        <v/>
+      </c>
+      <c r="E2" s="2">
         <f>[1]Fernanda!AC2</f>
-        <v>HRV</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
+        <v/>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>que é bom nada ne</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+    <row r="3">
+      <c r="A3" s="1" t="n">
         <v>44537</v>
       </c>
-      <c r="B3" t="str">
+      <c r="B3">
         <f>[1]Fernanda!Z3</f>
-        <v>JOAO</v>
-      </c>
-      <c r="C3" s="3">
+        <v/>
+      </c>
+      <c r="C3" s="3" t="n">
         <v>5544988045037</v>
       </c>
-      <c r="D3" t="str">
+      <c r="D3">
         <f>[1]Fernanda!AB3</f>
-        <v>GM</v>
-      </c>
-      <c r="E3" s="2" t="str">
+        <v/>
+      </c>
+      <c r="E3" s="2">
         <f>[1]Fernanda!AC3</f>
-        <v>ONIX</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
+        <v/>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>nao sei</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A2:A701">
-    <cfRule type="timePeriod" dxfId="0" priority="1" timePeriod="yesterday">
+    <cfRule dxfId="0" priority="1" timePeriod="yesterday" type="timePeriod">
       <formula>FLOOR(A2,1)=TODAY()-1</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins bottom="0.787401575" footer="0.31496062" header="0.31496062" left="0.511811024" right="0.511811024" top="0.787401575"/>
 </worksheet>
 </file>
</xml_diff>